<commit_message>
Changed "Hickmann Alves" name
</commit_message>
<xml_diff>
--- a/source/excel/nwsl-2016/nwsl-2016-was-orl-061816.xlsx
+++ b/source/excel/nwsl-2016/nwsl-2016-was-orl-061816.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/alfredo/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/alfredo/wosostats/source/excel/nwsl-2016/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -749,10 +749,10 @@
     <t>90+3</t>
   </si>
   <si>
-    <t>Hickmann-Alves (21)</t>
+    <t>passes.b.c</t>
   </si>
   <si>
-    <t>passes.b.c</t>
+    <t>Hickmann Alves (21)</t>
   </si>
 </sst>
 </file>
@@ -1317,7 +1317,7 @@
   <dimension ref="A1:T1415"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H16" sqref="H16:I16"/>
+      <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -2824,7 +2824,7 @@
         <v>136</v>
       </c>
       <c r="E25" s="13" t="s">
-        <v>239</v>
+        <v>240</v>
       </c>
       <c r="F25" s="14" t="s">
         <v>156</v>
@@ -2845,7 +2845,7 @@
         <v>136</v>
       </c>
       <c r="L25" s="13" t="s">
-        <v>239</v>
+        <v>240</v>
       </c>
       <c r="M25" s="2" t="s">
         <v>20</v>
@@ -5697,7 +5697,7 @@
         <v>20</v>
       </c>
       <c r="L71" s="1" t="s">
-        <v>239</v>
+        <v>240</v>
       </c>
       <c r="M71" s="2" t="s">
         <v>78</v>
@@ -6007,7 +6007,7 @@
         <v>20</v>
       </c>
       <c r="L76" s="1" t="s">
-        <v>239</v>
+        <v>240</v>
       </c>
       <c r="M76" s="2" t="s">
         <v>78</v>
@@ -6937,7 +6937,7 @@
         <v>20</v>
       </c>
       <c r="L91" s="1" t="s">
-        <v>239</v>
+        <v>240</v>
       </c>
       <c r="M91" s="2" t="s">
         <v>78</v>
@@ -7185,7 +7185,7 @@
         <v>20</v>
       </c>
       <c r="L95" s="1" t="s">
-        <v>239</v>
+        <v>240</v>
       </c>
       <c r="M95" s="2" t="s">
         <v>37</v>
@@ -7226,7 +7226,7 @@
         <v>20</v>
       </c>
       <c r="E96" s="1" t="s">
-        <v>239</v>
+        <v>240</v>
       </c>
       <c r="F96" s="2" t="s">
         <v>75</v>
@@ -7846,7 +7846,7 @@
         <v>20</v>
       </c>
       <c r="E106" s="1" t="s">
-        <v>239</v>
+        <v>240</v>
       </c>
       <c r="F106" s="2" t="s">
         <v>75</v>
@@ -8032,7 +8032,7 @@
         <v>20</v>
       </c>
       <c r="E109" s="1" t="s">
-        <v>239</v>
+        <v>240</v>
       </c>
       <c r="F109" s="2" t="s">
         <v>75</v>
@@ -8301,7 +8301,7 @@
         <v>20</v>
       </c>
       <c r="L113" s="1" t="s">
-        <v>239</v>
+        <v>240</v>
       </c>
       <c r="M113" s="2" t="s">
         <v>100</v>
@@ -8342,7 +8342,7 @@
         <v>20</v>
       </c>
       <c r="E114" s="1" t="s">
-        <v>239</v>
+        <v>240</v>
       </c>
       <c r="F114" s="2" t="s">
         <v>75</v>
@@ -9086,7 +9086,7 @@
         <v>20</v>
       </c>
       <c r="E126" s="1" t="s">
-        <v>239</v>
+        <v>240</v>
       </c>
       <c r="F126" s="2" t="s">
         <v>75</v>
@@ -10078,7 +10078,7 @@
         <v>20</v>
       </c>
       <c r="E142" s="1" t="s">
-        <v>239</v>
+        <v>240</v>
       </c>
       <c r="F142" s="2" t="s">
         <v>75</v>
@@ -11814,7 +11814,7 @@
         <v>20</v>
       </c>
       <c r="E170" s="1" t="s">
-        <v>239</v>
+        <v>240</v>
       </c>
       <c r="F170" s="2" t="s">
         <v>75</v>
@@ -12496,7 +12496,7 @@
         <v>20</v>
       </c>
       <c r="E181" s="1" t="s">
-        <v>239</v>
+        <v>240</v>
       </c>
       <c r="F181" s="2" t="s">
         <v>90</v>
@@ -12765,7 +12765,7 @@
         <v>20</v>
       </c>
       <c r="L185" s="1" t="s">
-        <v>239</v>
+        <v>240</v>
       </c>
       <c r="M185" s="2" t="s">
         <v>78</v>
@@ -13550,7 +13550,7 @@
         <v>20</v>
       </c>
       <c r="E198" s="1" t="s">
-        <v>239</v>
+        <v>240</v>
       </c>
       <c r="F198" s="2" t="s">
         <v>75</v>
@@ -14377,7 +14377,7 @@
         <v>20</v>
       </c>
       <c r="L211" s="1" t="s">
-        <v>239</v>
+        <v>240</v>
       </c>
       <c r="M211" s="2" t="s">
         <v>78</v>
@@ -17518,7 +17518,7 @@
         <v>20</v>
       </c>
       <c r="E262" s="1" t="s">
-        <v>239</v>
+        <v>240</v>
       </c>
       <c r="F262" s="2" t="s">
         <v>75</v>
@@ -17642,7 +17642,7 @@
         <v>20</v>
       </c>
       <c r="E264" s="1" t="s">
-        <v>239</v>
+        <v>240</v>
       </c>
       <c r="F264" s="2" t="s">
         <v>75</v>
@@ -19626,7 +19626,7 @@
         <v>20</v>
       </c>
       <c r="E296" s="1" t="s">
-        <v>239</v>
+        <v>240</v>
       </c>
       <c r="F296" s="2" t="s">
         <v>117</v>
@@ -19895,7 +19895,7 @@
         <v>20</v>
       </c>
       <c r="L300" s="1" t="s">
-        <v>239</v>
+        <v>240</v>
       </c>
       <c r="M300" s="2" t="s">
         <v>100</v>
@@ -19936,7 +19936,7 @@
         <v>20</v>
       </c>
       <c r="E301" s="1" t="s">
-        <v>239</v>
+        <v>240</v>
       </c>
       <c r="F301" s="2" t="s">
         <v>75</v>
@@ -20184,7 +20184,7 @@
         <v>20</v>
       </c>
       <c r="E305" s="1" t="s">
-        <v>239</v>
+        <v>240</v>
       </c>
       <c r="F305" s="2" t="s">
         <v>83</v>
@@ -20618,7 +20618,7 @@
         <v>20</v>
       </c>
       <c r="E312" s="1" t="s">
-        <v>239</v>
+        <v>240</v>
       </c>
       <c r="F312" s="2" t="s">
         <v>83</v>
@@ -23305,7 +23305,7 @@
         <v>20</v>
       </c>
       <c r="L355" s="1" t="s">
-        <v>239</v>
+        <v>240</v>
       </c>
       <c r="M355" s="2" t="s">
         <v>78</v>
@@ -23470,7 +23470,7 @@
         <v>20</v>
       </c>
       <c r="E358" s="1" t="s">
-        <v>239</v>
+        <v>240</v>
       </c>
       <c r="F358" s="2" t="s">
         <v>75</v>
@@ -26818,7 +26818,7 @@
         <v>20</v>
       </c>
       <c r="E412" s="1" t="s">
-        <v>239</v>
+        <v>240</v>
       </c>
       <c r="F412" s="2" t="s">
         <v>75</v>
@@ -27004,7 +27004,7 @@
         <v>20</v>
       </c>
       <c r="E415" s="1" t="s">
-        <v>239</v>
+        <v>240</v>
       </c>
       <c r="F415" s="2" t="s">
         <v>75</v>
@@ -27128,7 +27128,7 @@
         <v>20</v>
       </c>
       <c r="E417" s="1" t="s">
-        <v>239</v>
+        <v>240</v>
       </c>
       <c r="F417" s="2" t="s">
         <v>90</v>
@@ -28368,7 +28368,7 @@
         <v>20</v>
       </c>
       <c r="E437" s="1" t="s">
-        <v>239</v>
+        <v>240</v>
       </c>
       <c r="F437" s="2" t="s">
         <v>133</v>
@@ -28430,7 +28430,7 @@
         <v>20</v>
       </c>
       <c r="E438" s="1" t="s">
-        <v>239</v>
+        <v>240</v>
       </c>
       <c r="F438" s="2" t="s">
         <v>75</v>
@@ -28761,7 +28761,7 @@
         <v>20</v>
       </c>
       <c r="L443" s="1" t="s">
-        <v>239</v>
+        <v>240</v>
       </c>
       <c r="M443" s="2" t="s">
         <v>68</v>
@@ -29505,7 +29505,7 @@
         <v>20</v>
       </c>
       <c r="L455" s="1" t="s">
-        <v>239</v>
+        <v>240</v>
       </c>
       <c r="M455" s="2" t="s">
         <v>78</v>
@@ -32233,7 +32233,7 @@
         <v>20</v>
       </c>
       <c r="L499" s="1" t="s">
-        <v>239</v>
+        <v>240</v>
       </c>
       <c r="M499" s="2" t="s">
         <v>86</v>
@@ -34878,7 +34878,7 @@
         <v>20</v>
       </c>
       <c r="E542" s="1" t="s">
-        <v>239</v>
+        <v>240</v>
       </c>
       <c r="F542" s="2" t="s">
         <v>75</v>
@@ -35705,7 +35705,7 @@
         <v>20</v>
       </c>
       <c r="L555" s="1" t="s">
-        <v>239</v>
+        <v>240</v>
       </c>
       <c r="M555" s="2" t="s">
         <v>37</v>
@@ -36015,7 +36015,7 @@
         <v>20</v>
       </c>
       <c r="L560" s="1" t="s">
-        <v>239</v>
+        <v>240</v>
       </c>
       <c r="M560" s="2" t="s">
         <v>120</v>
@@ -36387,7 +36387,7 @@
         <v>20</v>
       </c>
       <c r="L566" s="1" t="s">
-        <v>239</v>
+        <v>240</v>
       </c>
       <c r="M566" s="2" t="s">
         <v>78</v>
@@ -37441,7 +37441,7 @@
         <v>20</v>
       </c>
       <c r="L583" s="1" t="s">
-        <v>239</v>
+        <v>240</v>
       </c>
       <c r="M583" s="2" t="s">
         <v>47</v>
@@ -37627,7 +37627,7 @@
         <v>20</v>
       </c>
       <c r="L586" s="1" t="s">
-        <v>239</v>
+        <v>240</v>
       </c>
       <c r="M586" s="2" t="s">
         <v>78</v>
@@ -38226,7 +38226,7 @@
         <v>20</v>
       </c>
       <c r="E596" s="1" t="s">
-        <v>239</v>
+        <v>240</v>
       </c>
       <c r="F596" s="2" t="s">
         <v>75</v>
@@ -38929,7 +38929,7 @@
         <v>20</v>
       </c>
       <c r="L607" s="1" t="s">
-        <v>239</v>
+        <v>240</v>
       </c>
       <c r="M607" s="2" t="s">
         <v>78</v>
@@ -39094,7 +39094,7 @@
         <v>20</v>
       </c>
       <c r="E610" s="1" t="s">
-        <v>239</v>
+        <v>240</v>
       </c>
       <c r="F610" s="2" t="s">
         <v>90</v>
@@ -39404,7 +39404,7 @@
         <v>20</v>
       </c>
       <c r="E615" s="1" t="s">
-        <v>239</v>
+        <v>240</v>
       </c>
       <c r="F615" s="2" t="s">
         <v>75</v>
@@ -39528,7 +39528,7 @@
         <v>20</v>
       </c>
       <c r="E617" s="1" t="s">
-        <v>239</v>
+        <v>240</v>
       </c>
       <c r="F617" s="2" t="s">
         <v>83</v>
@@ -42690,7 +42690,7 @@
         <v>20</v>
       </c>
       <c r="E668" s="1" t="s">
-        <v>239</v>
+        <v>240</v>
       </c>
       <c r="F668" s="2" t="s">
         <v>75</v>
@@ -43310,7 +43310,7 @@
         <v>20</v>
       </c>
       <c r="E678" s="1" t="s">
-        <v>239</v>
+        <v>240</v>
       </c>
       <c r="F678" s="2" t="s">
         <v>75</v>
@@ -44302,7 +44302,7 @@
         <v>20</v>
       </c>
       <c r="E694" s="1" t="s">
-        <v>239</v>
+        <v>240</v>
       </c>
       <c r="F694" s="2" t="s">
         <v>83</v>
@@ -45865,7 +45865,7 @@
         <v>136</v>
       </c>
       <c r="L731" s="1" t="s">
-        <v>239</v>
+        <v>240</v>
       </c>
       <c r="M731" s="28" t="s">
         <v>176</v>
@@ -46397,7 +46397,7 @@
         <v>136</v>
       </c>
       <c r="E748" s="1" t="s">
-        <v>239</v>
+        <v>240</v>
       </c>
       <c r="F748" s="28" t="s">
         <v>189</v>
@@ -46426,7 +46426,7 @@
         <v>136</v>
       </c>
       <c r="E749" s="1" t="s">
-        <v>239</v>
+        <v>240</v>
       </c>
       <c r="F749" s="28" t="s">
         <v>174</v>
@@ -46569,7 +46569,7 @@
         <v>216</v>
       </c>
       <c r="F753" s="28" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="G753" s="28"/>
       <c r="H753" s="28"/>
@@ -46767,7 +46767,7 @@
         <v>136</v>
       </c>
       <c r="L759" s="1" t="s">
-        <v>239</v>
+        <v>240</v>
       </c>
       <c r="M759" s="28" t="s">
         <v>176</v>
@@ -47560,7 +47560,7 @@
         <v>136</v>
       </c>
       <c r="L784" s="1" t="s">
-        <v>239</v>
+        <v>240</v>
       </c>
       <c r="M784" s="28" t="s">
         <v>176</v>
@@ -47873,7 +47873,7 @@
         <v>136</v>
       </c>
       <c r="E794" s="1" t="s">
-        <v>239</v>
+        <v>240</v>
       </c>
       <c r="F794" s="28" t="s">
         <v>189</v>
@@ -47902,7 +47902,7 @@
         <v>136</v>
       </c>
       <c r="E795" s="1" t="s">
-        <v>239</v>
+        <v>240</v>
       </c>
       <c r="F795" s="28" t="s">
         <v>215</v>
@@ -48222,7 +48222,7 @@
         <v>136</v>
       </c>
       <c r="E805" s="1" t="s">
-        <v>239</v>
+        <v>240</v>
       </c>
       <c r="F805" s="28" t="s">
         <v>179</v>
@@ -49140,7 +49140,7 @@
         <v>136</v>
       </c>
       <c r="E833" s="1" t="s">
-        <v>239</v>
+        <v>240</v>
       </c>
       <c r="F833" s="28" t="s">
         <v>189</v>
@@ -49169,7 +49169,7 @@
         <v>136</v>
       </c>
       <c r="E834" s="1" t="s">
-        <v>239</v>
+        <v>240</v>
       </c>
       <c r="F834" s="28" t="s">
         <v>174</v>
@@ -49495,7 +49495,7 @@
         <v>136</v>
       </c>
       <c r="E844" s="1" t="s">
-        <v>239</v>
+        <v>240</v>
       </c>
       <c r="F844" s="28" t="s">
         <v>204</v>
@@ -49675,7 +49675,7 @@
         <v>136</v>
       </c>
       <c r="L849" s="1" t="s">
-        <v>239</v>
+        <v>240</v>
       </c>
       <c r="M849" s="28" t="s">
         <v>190</v>
@@ -50885,7 +50885,7 @@
         <v>136</v>
       </c>
       <c r="E886" s="1" t="s">
-        <v>239</v>
+        <v>240</v>
       </c>
       <c r="F886" s="28" t="s">
         <v>174</v>
@@ -51644,7 +51644,7 @@
         <v>136</v>
       </c>
       <c r="E909" s="1" t="s">
-        <v>239</v>
+        <v>240</v>
       </c>
       <c r="F909" s="28" t="s">
         <v>174</v>
@@ -52243,7 +52243,7 @@
         <v>136</v>
       </c>
       <c r="L927" s="1" t="s">
-        <v>239</v>
+        <v>240</v>
       </c>
       <c r="M927" s="28" t="s">
         <v>220</v>
@@ -52812,7 +52812,7 @@
         <v>136</v>
       </c>
       <c r="E945" s="1" t="s">
-        <v>239</v>
+        <v>240</v>
       </c>
       <c r="F945" s="28" t="s">
         <v>172</v>
@@ -52913,7 +52913,7 @@
         <v>136</v>
       </c>
       <c r="E948" s="1" t="s">
-        <v>239</v>
+        <v>240</v>
       </c>
       <c r="F948" s="28" t="s">
         <v>172</v>
@@ -52973,7 +52973,7 @@
         <v>136</v>
       </c>
       <c r="E950" s="1" t="s">
-        <v>239</v>
+        <v>240</v>
       </c>
       <c r="F950" s="28" t="s">
         <v>174</v>
@@ -53339,7 +53339,7 @@
         <v>136</v>
       </c>
       <c r="L961" s="1" t="s">
-        <v>239</v>
+        <v>240</v>
       </c>
       <c r="M961" s="28" t="s">
         <v>204</v>
@@ -54697,7 +54697,7 @@
         <v>136</v>
       </c>
       <c r="E1004" s="1" t="s">
-        <v>239</v>
+        <v>240</v>
       </c>
       <c r="F1004" s="28" t="s">
         <v>174</v>
@@ -55267,7 +55267,7 @@
         <v>136</v>
       </c>
       <c r="E1022" s="1" t="s">
-        <v>239</v>
+        <v>240</v>
       </c>
       <c r="F1022" s="28" t="s">
         <v>172</v>
@@ -55339,7 +55339,7 @@
         <v>136</v>
       </c>
       <c r="E1024" s="1" t="s">
-        <v>239</v>
+        <v>240</v>
       </c>
       <c r="F1024" s="28" t="s">
         <v>174</v>
@@ -57026,7 +57026,7 @@
         <v>136</v>
       </c>
       <c r="E1077" s="1" t="s">
-        <v>239</v>
+        <v>240</v>
       </c>
       <c r="F1077" s="28" t="s">
         <v>174</v>
@@ -57324,7 +57324,7 @@
         <v>136</v>
       </c>
       <c r="L1086" s="1" t="s">
-        <v>239</v>
+        <v>240</v>
       </c>
       <c r="M1086" s="28" t="s">
         <v>204</v>
@@ -57823,7 +57823,7 @@
         <v>136</v>
       </c>
       <c r="E1102" s="1" t="s">
-        <v>239</v>
+        <v>240</v>
       </c>
       <c r="F1102" s="28" t="s">
         <v>179</v>
@@ -58091,7 +58091,7 @@
         <v>136</v>
       </c>
       <c r="E1110" s="1" t="s">
-        <v>239</v>
+        <v>240</v>
       </c>
       <c r="F1110" s="28" t="s">
         <v>174</v>
@@ -58196,7 +58196,7 @@
         <v>136</v>
       </c>
       <c r="E1113" s="1" t="s">
-        <v>239</v>
+        <v>240</v>
       </c>
       <c r="F1113" s="28" t="s">
         <v>174</v>
@@ -58388,7 +58388,7 @@
         <v>136</v>
       </c>
       <c r="E1119" s="1" t="s">
-        <v>239</v>
+        <v>240</v>
       </c>
       <c r="F1119" s="28" t="s">
         <v>179</v>
@@ -58557,7 +58557,7 @@
         <v>136</v>
       </c>
       <c r="E1124" s="1" t="s">
-        <v>239</v>
+        <v>240</v>
       </c>
       <c r="F1124" s="28" t="s">
         <v>174</v>
@@ -58954,7 +58954,7 @@
         <v>136</v>
       </c>
       <c r="L1136" s="1" t="s">
-        <v>239</v>
+        <v>240</v>
       </c>
       <c r="M1136" s="28" t="s">
         <v>176</v>
@@ -60194,7 +60194,7 @@
         <v>136</v>
       </c>
       <c r="E1175" s="1" t="s">
-        <v>239</v>
+        <v>240</v>
       </c>
       <c r="F1175" s="28" t="s">
         <v>172</v>
@@ -60264,7 +60264,7 @@
         <v>136</v>
       </c>
       <c r="E1177" s="1" t="s">
-        <v>239</v>
+        <v>240</v>
       </c>
       <c r="F1177" s="28" t="s">
         <v>179</v>
@@ -60328,7 +60328,7 @@
         <v>136</v>
       </c>
       <c r="E1179" s="1" t="s">
-        <v>239</v>
+        <v>240</v>
       </c>
       <c r="F1179" s="28" t="s">
         <v>174</v>
@@ -60726,7 +60726,7 @@
         <v>136</v>
       </c>
       <c r="E1191" s="1" t="s">
-        <v>239</v>
+        <v>240</v>
       </c>
       <c r="F1191" s="28" t="s">
         <v>189</v>
@@ -60755,7 +60755,7 @@
         <v>136</v>
       </c>
       <c r="E1192" s="1" t="s">
-        <v>239</v>
+        <v>240</v>
       </c>
       <c r="F1192" s="28" t="s">
         <v>174</v>
@@ -62416,7 +62416,7 @@
         <v>136</v>
       </c>
       <c r="L1244" s="1" t="s">
-        <v>239</v>
+        <v>240</v>
       </c>
       <c r="M1244" s="28" t="s">
         <v>217</v>
@@ -62438,7 +62438,7 @@
         <v>136</v>
       </c>
       <c r="E1245" s="1" t="s">
-        <v>239</v>
+        <v>240</v>
       </c>
       <c r="F1245" s="28" t="s">
         <v>189</v>
@@ -62467,7 +62467,7 @@
         <v>136</v>
       </c>
       <c r="E1246" s="1" t="s">
-        <v>239</v>
+        <v>240</v>
       </c>
       <c r="F1246" s="28" t="s">
         <v>174</v>
@@ -62659,7 +62659,7 @@
         <v>136</v>
       </c>
       <c r="E1252" s="1" t="s">
-        <v>239</v>
+        <v>240</v>
       </c>
       <c r="F1252" s="28" t="s">
         <v>174</v>
@@ -62826,7 +62826,7 @@
         <v>136</v>
       </c>
       <c r="E1257" s="1" t="s">
-        <v>239</v>
+        <v>240</v>
       </c>
       <c r="F1257" s="28" t="s">
         <v>189</v>
@@ -62855,7 +62855,7 @@
         <v>136</v>
       </c>
       <c r="E1258" s="1" t="s">
-        <v>239</v>
+        <v>240</v>
       </c>
       <c r="F1258" s="28" t="s">
         <v>172</v>
@@ -63082,7 +63082,7 @@
         <v>136</v>
       </c>
       <c r="E1265" s="1" t="s">
-        <v>239</v>
+        <v>240</v>
       </c>
       <c r="F1265" s="28" t="s">
         <v>172</v>
@@ -63387,7 +63387,7 @@
         <v>136</v>
       </c>
       <c r="E1274" s="1" t="s">
-        <v>239</v>
+        <v>240</v>
       </c>
       <c r="F1274" s="28" t="s">
         <v>189</v>
@@ -63416,7 +63416,7 @@
         <v>136</v>
       </c>
       <c r="E1275" s="1" t="s">
-        <v>239</v>
+        <v>240</v>
       </c>
       <c r="F1275" s="28" t="s">
         <v>174</v>
@@ -63719,7 +63719,7 @@
         <v>136</v>
       </c>
       <c r="E1284" s="1" t="s">
-        <v>239</v>
+        <v>240</v>
       </c>
       <c r="F1284" s="28" t="s">
         <v>179</v>
@@ -64002,7 +64002,7 @@
         <v>136</v>
       </c>
       <c r="E1293" s="1" t="s">
-        <v>239</v>
+        <v>240</v>
       </c>
       <c r="F1293" s="28" t="s">
         <v>174</v>
@@ -64066,7 +64066,7 @@
         <v>136</v>
       </c>
       <c r="E1295" s="1" t="s">
-        <v>239</v>
+        <v>240</v>
       </c>
       <c r="F1295" s="28" t="s">
         <v>206</v>
@@ -64095,7 +64095,7 @@
         <v>136</v>
       </c>
       <c r="E1296" s="1" t="s">
-        <v>239</v>
+        <v>240</v>
       </c>
       <c r="F1296" s="28" t="s">
         <v>174</v>
@@ -64188,7 +64188,7 @@
         <v>136</v>
       </c>
       <c r="E1299" s="1" t="s">
-        <v>239</v>
+        <v>240</v>
       </c>
       <c r="F1299" s="28" t="s">
         <v>174</v>
@@ -64743,7 +64743,7 @@
         <v>136</v>
       </c>
       <c r="E1316" s="1" t="s">
-        <v>239</v>
+        <v>240</v>
       </c>
       <c r="F1316" s="28" t="s">
         <v>179</v>
@@ -64902,7 +64902,7 @@
         <v>136</v>
       </c>
       <c r="E1321" s="1" t="s">
-        <v>239</v>
+        <v>240</v>
       </c>
       <c r="F1321" s="28" t="s">
         <v>174</v>
@@ -65127,7 +65127,7 @@
         <v>136</v>
       </c>
       <c r="E1328" s="1" t="s">
-        <v>239</v>
+        <v>240</v>
       </c>
       <c r="F1328" s="28" t="s">
         <v>174</v>
@@ -65762,7 +65762,7 @@
         <v>136</v>
       </c>
       <c r="E1347" s="1" t="s">
-        <v>239</v>
+        <v>240</v>
       </c>
       <c r="F1347" s="28" t="s">
         <v>174</v>
@@ -65963,7 +65963,7 @@
         <v>136</v>
       </c>
       <c r="L1353" s="1" t="s">
-        <v>239</v>
+        <v>240</v>
       </c>
       <c r="M1353" s="28" t="s">
         <v>204</v>
@@ -66539,7 +66539,7 @@
         <v>136</v>
       </c>
       <c r="L1371" s="1" t="s">
-        <v>239</v>
+        <v>240</v>
       </c>
       <c r="M1371" s="29" t="s">
         <v>176</v>
@@ -66722,7 +66722,7 @@
         <v>136</v>
       </c>
       <c r="L1376" s="1" t="s">
-        <v>239</v>
+        <v>240</v>
       </c>
       <c r="M1376" s="28" t="s">
         <v>176</v>
@@ -67029,7 +67029,7 @@
         <v>136</v>
       </c>
       <c r="E1386" s="1" t="s">
-        <v>239</v>
+        <v>240</v>
       </c>
       <c r="F1386" s="28" t="s">
         <v>179</v>
@@ -67830,7 +67830,7 @@
         <v>136</v>
       </c>
       <c r="L1410" s="1" t="s">
-        <v>239</v>
+        <v>240</v>
       </c>
       <c r="M1410" s="28" t="s">
         <v>204</v>

</xml_diff>